<commit_message>
change k1 - 0.55 to 0.8
</commit_message>
<xml_diff>
--- a/Train/Files/Стоимость.xlsx
+++ b/Train/Files/Стоимость.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\Abbosbek\Documents\Visual Studio 2022\Projects\Abbossbek\Train-new\Train\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\abbosbek\Documents\Visual Studio 2022\Projects\Abbossbek\Train-new\Train\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3282B47-3059-4AC6-83DC-A905897F0D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914EE90-EA76-4FC1-A1A1-17FAAA44057A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="3915" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="9" r:id="rId1"/>
@@ -13110,6 +13110,9 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -13193,9 +13196,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -13481,7 +13481,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13524,7 +13524,7 @@
         <v>631</v>
       </c>
       <c r="F2">
-        <v>0.55000000000000004</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -13571,7 +13571,7 @@
       <c r="C5" s="57">
         <v>8</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="64" t="s">
         <v>997</v>
       </c>
       <c r="F5">
@@ -27080,18 +27080,18 @@
       </c>
     </row>
     <row r="73" spans="1:61" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="64" t="s">
+      <c r="A73" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="B73" s="65"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="66"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="66"/>
+      <c r="J73" s="67"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
@@ -40733,69 +40733,69 @@
       </c>
     </row>
     <row r="73" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A73" s="69" t="s">
+      <c r="A73" s="70" t="s">
         <v>975</v>
       </c>
-      <c r="B73" s="67"/>
-      <c r="C73" s="67"/>
-      <c r="D73" s="67"/>
-      <c r="E73" s="67"/>
-      <c r="F73" s="67"/>
-      <c r="G73" s="67"/>
-      <c r="H73" s="67"/>
-      <c r="I73" s="67"/>
-      <c r="J73" s="68"/>
-      <c r="K73" s="67"/>
-      <c r="L73" s="67"/>
-      <c r="M73" s="67"/>
-      <c r="N73" s="67"/>
-      <c r="O73" s="67"/>
-      <c r="P73" s="67"/>
-      <c r="Q73" s="67"/>
-      <c r="R73" s="67"/>
-      <c r="S73" s="68"/>
-      <c r="T73" s="67"/>
-      <c r="U73" s="67"/>
-      <c r="V73" s="67"/>
-      <c r="W73" s="67"/>
-      <c r="X73" s="67"/>
-      <c r="Y73" s="67"/>
-      <c r="Z73" s="67"/>
-      <c r="AA73" s="67"/>
-      <c r="AB73" s="68"/>
-      <c r="AC73" s="67"/>
-      <c r="AD73" s="67"/>
-      <c r="AE73" s="67"/>
-      <c r="AF73" s="67"/>
-      <c r="AG73" s="67"/>
-      <c r="AH73" s="67"/>
-      <c r="AI73" s="67"/>
-      <c r="AJ73" s="67"/>
-      <c r="AK73" s="68"/>
-      <c r="AL73" s="67"/>
-      <c r="AM73" s="67"/>
-      <c r="AN73" s="67"/>
-      <c r="AO73" s="67"/>
-      <c r="AP73" s="67"/>
-      <c r="AQ73" s="67"/>
-      <c r="AR73" s="67"/>
-      <c r="AS73" s="67"/>
-      <c r="AT73" s="68"/>
-      <c r="AU73" s="67"/>
-      <c r="AV73" s="67"/>
-      <c r="AW73" s="67"/>
-      <c r="AX73" s="67"/>
-      <c r="AY73" s="67"/>
-      <c r="AZ73" s="67"/>
-      <c r="BA73" s="67"/>
-      <c r="BB73" s="67"/>
-      <c r="BC73" s="68"/>
-      <c r="BD73" s="67"/>
-      <c r="BE73" s="67"/>
-      <c r="BF73" s="67"/>
-      <c r="BG73" s="67"/>
-      <c r="BH73" s="67"/>
-      <c r="BI73" s="68"/>
+      <c r="B73" s="68"/>
+      <c r="C73" s="68"/>
+      <c r="D73" s="68"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="68"/>
+      <c r="G73" s="68"/>
+      <c r="H73" s="68"/>
+      <c r="I73" s="68"/>
+      <c r="J73" s="69"/>
+      <c r="K73" s="68"/>
+      <c r="L73" s="68"/>
+      <c r="M73" s="68"/>
+      <c r="N73" s="68"/>
+      <c r="O73" s="68"/>
+      <c r="P73" s="68"/>
+      <c r="Q73" s="68"/>
+      <c r="R73" s="68"/>
+      <c r="S73" s="69"/>
+      <c r="T73" s="68"/>
+      <c r="U73" s="68"/>
+      <c r="V73" s="68"/>
+      <c r="W73" s="68"/>
+      <c r="X73" s="68"/>
+      <c r="Y73" s="68"/>
+      <c r="Z73" s="68"/>
+      <c r="AA73" s="68"/>
+      <c r="AB73" s="69"/>
+      <c r="AC73" s="68"/>
+      <c r="AD73" s="68"/>
+      <c r="AE73" s="68"/>
+      <c r="AF73" s="68"/>
+      <c r="AG73" s="68"/>
+      <c r="AH73" s="68"/>
+      <c r="AI73" s="68"/>
+      <c r="AJ73" s="68"/>
+      <c r="AK73" s="69"/>
+      <c r="AL73" s="68"/>
+      <c r="AM73" s="68"/>
+      <c r="AN73" s="68"/>
+      <c r="AO73" s="68"/>
+      <c r="AP73" s="68"/>
+      <c r="AQ73" s="68"/>
+      <c r="AR73" s="68"/>
+      <c r="AS73" s="68"/>
+      <c r="AT73" s="69"/>
+      <c r="AU73" s="68"/>
+      <c r="AV73" s="68"/>
+      <c r="AW73" s="68"/>
+      <c r="AX73" s="68"/>
+      <c r="AY73" s="68"/>
+      <c r="AZ73" s="68"/>
+      <c r="BA73" s="68"/>
+      <c r="BB73" s="68"/>
+      <c r="BC73" s="69"/>
+      <c r="BD73" s="68"/>
+      <c r="BE73" s="68"/>
+      <c r="BF73" s="68"/>
+      <c r="BG73" s="68"/>
+      <c r="BH73" s="68"/>
+      <c r="BI73" s="69"/>
     </row>
     <row r="74" spans="1:61" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
@@ -41013,82 +41013,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="71" t="s">
         <v>634</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="69" t="s">
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="69" t="s">
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="69" t="s">
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="69" t="s">
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="69"/>
+      <c r="AD1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="67"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="69" t="s">
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="69"/>
+      <c r="AK1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="68"/>
-      <c r="AR1" s="69" t="s">
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="68"/>
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
+      <c r="AQ1" s="69"/>
+      <c r="AR1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="AS1" s="67"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="67"/>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="67"/>
-      <c r="AX1" s="68"/>
-      <c r="AY1" s="69" t="s">
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="68"/>
+      <c r="AU1" s="68"/>
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="69"/>
+      <c r="AY1" s="70" t="s">
         <v>636</v>
       </c>
-      <c r="AZ1" s="68"/>
-      <c r="BA1" s="70" t="s">
+      <c r="AZ1" s="69"/>
+      <c r="BA1" s="71" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="2" spans="1:53" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="71"/>
+      <c r="A2" s="72"/>
       <c r="B2" s="24" t="s">
         <v>637</v>
       </c>
@@ -41242,7 +41242,7 @@
       <c r="AZ2" s="24" t="s">
         <v>687</v>
       </c>
-      <c r="BA2" s="71"/>
+      <c r="BA2" s="72"/>
     </row>
     <row r="3" spans="1:53" ht="14.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24"/>
@@ -46853,18 +46853,18 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="76" t="s">
         <v>748</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
       <c r="M1" s="32"/>
@@ -46909,18 +46909,18 @@
       <c r="AZ1" s="32"/>
     </row>
     <row r="2" spans="1:52" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>749</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
       <c r="M2" s="32"/>
@@ -46965,75 +46965,75 @@
       <c r="AZ2" s="32"/>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="78" t="s">
         <v>750</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="73" t="s">
         <v>696</v>
       </c>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="72" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="73" t="s">
         <v>696</v>
       </c>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="73"/>
-      <c r="P3" s="73"/>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="72" t="s">
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="75"/>
+      <c r="T3" s="73" t="s">
         <v>696</v>
       </c>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="73"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="73"/>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="72" t="s">
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="73" t="s">
         <v>696</v>
       </c>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="73"/>
-      <c r="AH3" s="73"/>
-      <c r="AI3" s="73"/>
-      <c r="AJ3" s="73"/>
-      <c r="AK3" s="74"/>
-      <c r="AL3" s="72" t="s">
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="74"/>
+      <c r="AF3" s="74"/>
+      <c r="AG3" s="74"/>
+      <c r="AH3" s="74"/>
+      <c r="AI3" s="74"/>
+      <c r="AJ3" s="74"/>
+      <c r="AK3" s="75"/>
+      <c r="AL3" s="73" t="s">
         <v>696</v>
       </c>
-      <c r="AM3" s="73"/>
-      <c r="AN3" s="73"/>
-      <c r="AO3" s="73"/>
-      <c r="AP3" s="73"/>
-      <c r="AQ3" s="73"/>
-      <c r="AR3" s="73"/>
-      <c r="AS3" s="73"/>
-      <c r="AT3" s="74"/>
-      <c r="AU3" s="72" t="s">
+      <c r="AM3" s="74"/>
+      <c r="AN3" s="74"/>
+      <c r="AO3" s="74"/>
+      <c r="AP3" s="74"/>
+      <c r="AQ3" s="74"/>
+      <c r="AR3" s="74"/>
+      <c r="AS3" s="74"/>
+      <c r="AT3" s="75"/>
+      <c r="AU3" s="73" t="s">
         <v>696</v>
       </c>
-      <c r="AV3" s="73"/>
-      <c r="AW3" s="73"/>
-      <c r="AX3" s="73"/>
-      <c r="AY3" s="73"/>
-      <c r="AZ3" s="74"/>
+      <c r="AV3" s="74"/>
+      <c r="AW3" s="74"/>
+      <c r="AX3" s="74"/>
+      <c r="AY3" s="74"/>
+      <c r="AZ3" s="75"/>
     </row>
     <row r="4" spans="1:52" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="78"/>
+      <c r="A4" s="79"/>
       <c r="B4" s="33" t="s">
         <v>751</v>
       </c>
@@ -51955,17 +51955,17 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:61" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>802</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
       <c r="J1" s="38"/>
       <c r="K1" s="38"/>
       <c r="L1" s="38"/>
@@ -52020,17 +52020,17 @@
       <c r="BI1" s="38"/>
     </row>
     <row r="2" spans="1:61" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="81" t="s">
         <v>803</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
       <c r="J2" s="38"/>
       <c r="K2" s="38"/>
       <c r="L2" s="38"/>
@@ -52085,18 +52085,18 @@
       <c r="BI2" s="38"/>
     </row>
     <row r="3" spans="1:61" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="82" t="s">
         <v>804</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="84" t="s">
         <v>805</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="86"/>
       <c r="I3" s="38"/>
       <c r="J3" s="38"/>
       <c r="K3" s="38"/>
@@ -52152,7 +52152,7 @@
       <c r="BI3" s="38"/>
     </row>
     <row r="4" spans="1:61" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="82"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="39" t="s">
         <v>806</v>
       </c>
@@ -54579,30 +54579,30 @@
       <c r="A1" s="43" t="s">
         <v>867</v>
       </c>
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="87" t="s">
         <v>868</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="89" t="s">
         <v>696</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
       <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="88"/>
+      <c r="A3" s="89"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44" t="s">
         <v>869</v>
@@ -54622,7 +54622,7 @@
       <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="88"/>
+      <c r="A4" s="89"/>
       <c r="B4" s="45">
         <v>93</v>
       </c>
@@ -55889,33 +55889,33 @@
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>925</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="71" t="s">
         <v>696</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>926</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="69"/>
       <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="91"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="24" t="s">
         <v>927</v>
       </c>
@@ -55937,19 +55937,19 @@
       <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="91"/>
-      <c r="B4" s="69" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="70" t="s">
         <v>928</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
+      <c r="A5" s="72"/>
       <c r="B5" s="29">
         <v>99</v>
       </c>

</xml_diff>